<commit_message>
added verification of words
</commit_message>
<xml_diff>
--- a/experimental_design/Design.xlsx
+++ b/experimental_design/Design.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="115">
   <si>
     <t>Token</t>
   </si>
@@ -91,28 +91,28 @@
     <t>ChangedIndexS2</t>
   </si>
   <si>
-    <t>reh</t>
-  </si>
-  <si>
-    <t>dehuc</t>
-  </si>
-  <si>
-    <t>cehidful</t>
-  </si>
-  <si>
-    <t>precehider</t>
-  </si>
-  <si>
-    <t>deprereh</t>
-  </si>
-  <si>
-    <t>irsableful</t>
-  </si>
-  <si>
-    <t>deifufulable</t>
-  </si>
-  <si>
-    <t>inunifuion</t>
+    <t>sar</t>
+  </si>
+  <si>
+    <t>presetet</t>
+  </si>
+  <si>
+    <t>seteter</t>
+  </si>
+  <si>
+    <t>desetetful</t>
+  </si>
+  <si>
+    <t>uninsut</t>
+  </si>
+  <si>
+    <t>owkiableful</t>
+  </si>
+  <si>
+    <t>deawtioner</t>
+  </si>
+  <si>
+    <t>predemetful</t>
   </si>
   <si>
     <t>r</t>
@@ -139,64 +139,76 @@
     <t>pprs</t>
   </si>
   <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>pre</t>
+  </si>
+  <si>
     <t>de</t>
   </si>
   <si>
     <t>in</t>
   </si>
   <si>
-    <t>pre</t>
-  </si>
-  <si>
-    <t>un</t>
-  </si>
-  <si>
-    <t>huc</t>
-  </si>
-  <si>
-    <t>cehid</t>
-  </si>
-  <si>
-    <t>irs</t>
-  </si>
-  <si>
-    <t>ifu</t>
+    <t>setet</t>
+  </si>
+  <si>
+    <t>sut</t>
+  </si>
+  <si>
+    <t>owki</t>
+  </si>
+  <si>
+    <t>awt</t>
+  </si>
+  <si>
+    <t>met</t>
+  </si>
+  <si>
+    <t>er</t>
   </si>
   <si>
     <t>ful</t>
   </si>
   <si>
-    <t>er</t>
-  </si>
-  <si>
     <t>able</t>
   </si>
   <si>
     <t>ion</t>
   </si>
   <si>
-    <t>ehr</t>
-  </si>
-  <si>
-    <t>educh</t>
-  </si>
-  <si>
-    <t>hidceufl</t>
-  </si>
-  <si>
-    <t>erpedhcire</t>
-  </si>
-  <si>
-    <t>edeprhre</t>
-  </si>
-  <si>
-    <t>rsilebaufl</t>
-  </si>
-  <si>
-    <t>eduiflfuabel</t>
-  </si>
-  <si>
-    <t>ninuiufoni</t>
+    <t>asr</t>
+  </si>
+  <si>
+    <t>erpstete</t>
+  </si>
+  <si>
+    <t>etsetre</t>
+  </si>
+  <si>
+    <t>edtsetelfu</t>
+  </si>
+  <si>
+    <t>nunitsu</t>
+  </si>
+  <si>
+    <t>ikowblaeulf</t>
+  </si>
+  <si>
+    <t>edwatoinre</t>
+  </si>
+  <si>
+    <t>rpeedtemlfu</t>
+  </si>
+  <si>
+    <t>nu</t>
+  </si>
+  <si>
+    <t>rpe</t>
+  </si>
+  <si>
+    <t>erp</t>
   </si>
   <si>
     <t>ed</t>
@@ -205,118 +217,106 @@
     <t>ni</t>
   </si>
   <si>
-    <t>erp</t>
-  </si>
-  <si>
-    <t>epr</t>
-  </si>
-  <si>
-    <t>nu</t>
-  </si>
-  <si>
-    <t>uch</t>
-  </si>
-  <si>
-    <t>hidce</t>
-  </si>
-  <si>
-    <t>edhci</t>
-  </si>
-  <si>
-    <t>hre</t>
-  </si>
-  <si>
-    <t>rsi</t>
-  </si>
-  <si>
-    <t>uif</t>
-  </si>
-  <si>
-    <t>iuf</t>
-  </si>
-  <si>
-    <t>ufl</t>
+    <t>stete</t>
+  </si>
+  <si>
+    <t>etset</t>
+  </si>
+  <si>
+    <t>tsete</t>
+  </si>
+  <si>
+    <t>tsu</t>
+  </si>
+  <si>
+    <t>ikow</t>
+  </si>
+  <si>
+    <t>wat</t>
+  </si>
+  <si>
+    <t>tem</t>
   </si>
   <si>
     <t>re</t>
   </si>
   <si>
-    <t>leba</t>
-  </si>
-  <si>
     <t>lfu</t>
   </si>
   <si>
-    <t>oni</t>
-  </si>
-  <si>
-    <t>abel</t>
-  </si>
-  <si>
-    <t>teprereh</t>
-  </si>
-  <si>
-    <t>irunifuion</t>
-  </si>
-  <si>
-    <t>dohuc</t>
-  </si>
-  <si>
-    <t>pricehider</t>
-  </si>
-  <si>
-    <t>depmereh</t>
-  </si>
-  <si>
-    <t>doifufulable</t>
-  </si>
-  <si>
-    <t>inonifuion</t>
-  </si>
-  <si>
-    <t>meh</t>
-  </si>
-  <si>
-    <t>dehac</t>
-  </si>
-  <si>
-    <t>cahidful</t>
-  </si>
-  <si>
-    <t>precehiter</t>
-  </si>
-  <si>
-    <t>deprerih</t>
-  </si>
-  <si>
-    <t>ijsableful</t>
-  </si>
-  <si>
-    <t>deisufulable</t>
-  </si>
-  <si>
-    <t>inunifaion</t>
-  </si>
-  <si>
-    <t>cehidfil</t>
-  </si>
-  <si>
-    <t>precehidur</t>
-  </si>
-  <si>
-    <t>irsagleful</t>
-  </si>
-  <si>
-    <t>deifuculable</t>
-  </si>
-  <si>
-    <t>inunifuior</t>
-  </si>
-  <si>
-    <t>irsablefol</t>
-  </si>
-  <si>
-    <t>deifufulablo</t>
+    <t>blae</t>
+  </si>
+  <si>
+    <t>oin</t>
+  </si>
+  <si>
+    <t>ulf</t>
+  </si>
+  <si>
+    <t>ulinsut</t>
+  </si>
+  <si>
+    <t>tredemetful</t>
+  </si>
+  <si>
+    <t>sresetet</t>
+  </si>
+  <si>
+    <t>dosetetful</t>
+  </si>
+  <si>
+    <t>unilsut</t>
+  </si>
+  <si>
+    <t>seawtioner</t>
+  </si>
+  <si>
+    <t>predametful</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>presotet</t>
+  </si>
+  <si>
+    <t>teteter</t>
+  </si>
+  <si>
+    <t>degetetful</t>
+  </si>
+  <si>
+    <t>uninset</t>
+  </si>
+  <si>
+    <t>iwkiableful</t>
+  </si>
+  <si>
+    <t>deiwtioner</t>
+  </si>
+  <si>
+    <t>predemotful</t>
+  </si>
+  <si>
+    <t>setetor</t>
+  </si>
+  <si>
+    <t>desetetfuy</t>
+  </si>
+  <si>
+    <t>owkiebleful</t>
+  </si>
+  <si>
+    <t>deawtiorer</t>
+  </si>
+  <si>
+    <t>predemetfel</t>
+  </si>
+  <si>
+    <t>owkiablefur</t>
+  </si>
+  <si>
+    <t>deawtionew</t>
   </si>
   <si>
     <t>Prefix</t>
@@ -334,19 +334,16 @@
     <t>all</t>
   </si>
   <si>
-    <t>bogi</t>
-  </si>
-  <si>
-    <t>otos</t>
-  </si>
-  <si>
-    <t>olva</t>
-  </si>
-  <si>
-    <t>yemd</t>
-  </si>
-  <si>
-    <t>tar</t>
+    <t>upi</t>
+  </si>
+  <si>
+    <t>boha</t>
+  </si>
+  <si>
+    <t>eget</t>
+  </si>
+  <si>
+    <t>rers</t>
   </si>
   <si>
     <t>Suffix</t>
@@ -816,16 +813,16 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q2" t="s">
         <v>85</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -836,22 +833,22 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="L3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P3" t="s">
         <v>80</v>
@@ -860,7 +857,7 @@
         <v>86</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <v>1</v>
@@ -874,22 +871,22 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q4" t="s">
         <v>87</v>
@@ -898,10 +895,10 @@
         <v>93</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -915,25 +912,25 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P5" t="s">
         <v>81</v>
@@ -945,13 +942,13 @@
         <v>94</v>
       </c>
       <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>2</v>
-      </c>
-      <c r="V5">
-        <v>4</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -965,25 +962,25 @@
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O6" t="s">
         <v>78</v>
@@ -995,7 +992,7 @@
         <v>89</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <v>1</v>
@@ -1015,25 +1012,25 @@
         <v>46</v>
       </c>
       <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
       <c r="H7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="Q7" t="s">
         <v>90</v>
@@ -1045,13 +1042,13 @@
         <v>98</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1062,34 +1059,34 @@
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="P8" t="s">
         <v>83</v>
@@ -1104,16 +1101,16 @@
         <v>99</v>
       </c>
       <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>2</v>
+      </c>
+      <c r="X8">
         <v>1</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1127,31 +1124,31 @@
         <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K9" t="s">
         <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O9" t="s">
         <v>79</v>
@@ -1166,16 +1163,16 @@
         <v>97</v>
       </c>
       <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
         <v>1</v>
       </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
       <c r="V9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1207,7 +1204,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>104</v>
@@ -1221,7 +1218,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>104</v>
@@ -1235,7 +1232,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>104</v>
@@ -1249,7 +1246,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>104</v>
@@ -1281,37 +1278,37 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -1321,12 +1318,12 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1344,27 +1341,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2">
         <v>0.35</v>
@@ -1372,13 +1369,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3">
         <v>0.25</v>
@@ -1386,13 +1383,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4">
         <v>0.2</v>
@@ -1403,10 +1400,10 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5">
         <v>0.2</v>

</xml_diff>